<commit_message>
Update Test Case Workbook
</commit_message>
<xml_diff>
--- a/TestCases/MiniMilestone_TestCases.xlsx
+++ b/TestCases/MiniMilestone_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dabde\Google Drive (abdulazd@mcmaster.ca)\Extracurriculars\IBEHS TA 2020 Fall\Autograder\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E9C7C8-2947-4417-B924-658D51833FA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927CAD6B-2384-4989-B247-2EF6EAD5BE6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="87">
   <si>
     <t>Guidelines for Inputs</t>
   </si>
@@ -35,6 +35,9 @@
     <t>TODO: Change sheet font to Courier</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
     <t>Student</t>
   </si>
   <si>
@@ -44,13 +47,199 @@
     <t>Outputs</t>
   </si>
   <si>
+    <t>output_speed(40,4+4/9)</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>output_speed(42,4+2/3)</t>
+  </si>
+  <si>
+    <t>output_speed(45,5)</t>
+  </si>
+  <si>
+    <t>motor_rev(4+4/9)</t>
+  </si>
+  <si>
     <t>B</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>1.1111111111111112</t>
+  </si>
+  <si>
+    <t>motor_rev(7+7/9)</t>
+  </si>
+  <si>
+    <t>1.9444444444444444</t>
+  </si>
+  <si>
+    <t>motor_rev(5+1/3)</t>
+  </si>
+  <si>
+    <t>1.3333333333333333</t>
+  </si>
+  <si>
+    <t>calc_xy_pos(45)</t>
+  </si>
+  <si>
+    <t>[-25.456, 10.544]</t>
+  </si>
+  <si>
+    <t>calc_xy_pos(20)</t>
+  </si>
+  <si>
+    <t>[-33.829, 23.687]</t>
+  </si>
+  <si>
+    <t>calc_xy_pos(90)</t>
+  </si>
+  <si>
+    <t>[-0.0, 0.0]</t>
+  </si>
+  <si>
+    <t>calc_elapsed_time(40,4+4/9)</t>
+  </si>
+  <si>
+    <t>1.6666666666666667</t>
+  </si>
+  <si>
+    <t>calc_elapsed_time(42,4+2/3)</t>
+  </si>
+  <si>
+    <t>1.666666666666667</t>
+  </si>
+  <si>
+    <t>calc_elapsed_time(45,5)</t>
+  </si>
+  <si>
+    <t>calc_GR([12,30,32],[12,13,13,20])</t>
+  </si>
+  <si>
+    <t>4.444444444444445</t>
+  </si>
+  <si>
+    <t>calc_GR([12,18,36],[12,20,20])</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>calc_GR([12,22,28],[12,12,12,24])</t>
+  </si>
+  <si>
+    <t>4.666666666666667</t>
+  </si>
+  <si>
+    <t>calc_PD([12,30,32],1)</t>
+  </si>
+  <si>
+    <t>[12, 30, 32]</t>
+  </si>
+  <si>
+    <t>calc_PD([12,30,32],2)</t>
+  </si>
+  <si>
+    <t>[24, 60, 64]</t>
+  </si>
+  <si>
+    <t>calc_PD([12,22,28],1)</t>
+  </si>
+  <si>
+    <t>[12, 22, 28]</t>
+  </si>
+  <si>
+    <t>calc_CD([12,30,32])</t>
+  </si>
+  <si>
+    <t>52.0</t>
+  </si>
+  <si>
+    <t>calc_CD([12,13,13,20])</t>
+  </si>
+  <si>
+    <t>42.0</t>
+  </si>
+  <si>
+    <t>calc_CD([12,20,20])</t>
+  </si>
+  <si>
+    <t>36.0</t>
+  </si>
+  <si>
+    <t>calc_incr_pos()</t>
+  </si>
+  <si>
+    <t>[[-36.0, 36.0], [-35.45307910843949, 29.74866560399051], [-33.828934348292705, 23.687274840275926], [-31.176914536239792, 18.000000000000004], [-27.577599952283208, 12.859646051284585], [-23.14035394871542, 8.422400047716792], [-18.000000000000004, 4.823085463760211], [-12.312725159724078, 2.171065651707302], [-6.251334396009495, 0.5469208915605108], [-2.204364238465236e-15, 0.0]]</t>
+  </si>
+  <si>
+    <t>verify_gear_ratio(4+4/9,[12,20,32],[12,13,13,20],[12,20,20])</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>verify_gear_ratio(4+4/9,[12,20,32],[12,13,13,20],[12,20,99])</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>verify_gear_ratio(4+4/9,[12,20,32],[12,13,13,99],[12,20,20])</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>verify_gear_ratio(4+4/9,[12,20,32],[12,13,13,99],[12,99,99])</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>verify_center_distance(1,[12,20,32],[12,13,13,20],[12,20,20])</t>
+  </si>
+  <si>
+    <t>verify_center_distance(1,[12,20,32],[12,13,13,20],[12,99,20])</t>
+  </si>
+  <si>
+    <t>verify_center_distance(1,[12,20,32],[12,13,99,20],[12,20,20])</t>
+  </si>
+  <si>
+    <t>verify_center_distance(1,[12,20,99],[12,13,13,20],[12,20,20])</t>
+  </si>
+  <si>
+    <t>verify_center_distance(1,[12,20,32],[12,13,99,20],[12,99,20])</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>verify_center_distance(1,[12,20,99],[12,13,13,20],[12,99,20])</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>verify_center_distance(1,[12,20,99],[12,13,99,20],[12,20,20])</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>verify_center_distance(1,[12,20,99],[12,13,99,20],[12,99,20])</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>verify_center_distance(2,[12,20,32],[12,13,13,20],[12,20,20])</t>
+  </si>
+  <si>
+    <t>verify_center_distance(2,[6,10,16],[6,6.5,6.5,10],[6,10,10])</t>
   </si>
   <si>
     <t>Constructor</t>
@@ -96,121 +285,13 @@
   </si>
   <si>
     <t>test_obj.other_method(1.5)</t>
-  </si>
-  <si>
-    <t>output_speed(40,4+4/9)</t>
-  </si>
-  <si>
-    <t>output_speed(42,4+2/3)</t>
-  </si>
-  <si>
-    <t>output_speed(45,5)</t>
-  </si>
-  <si>
-    <t>motor_rev(4+4/9)</t>
-  </si>
-  <si>
-    <t>motor_rev(7+7/9)</t>
-  </si>
-  <si>
-    <t>motor_rev(5+1/3)</t>
-  </si>
-  <si>
-    <t>calc_xy_pos(45)</t>
-  </si>
-  <si>
-    <t>calc_xy_pos(20)</t>
-  </si>
-  <si>
-    <t>calc_xy_pos(90)</t>
-  </si>
-  <si>
-    <t>calc_elapsed_time(40,4+4/9)</t>
-  </si>
-  <si>
-    <t>calc_elapsed_time(42,4+2/3)</t>
-  </si>
-  <si>
-    <t>calc_elapsed_time(45,5)</t>
-  </si>
-  <si>
-    <t>calc_GR([12,30,32])</t>
-  </si>
-  <si>
-    <t>calc_GR([12,18,36])</t>
-  </si>
-  <si>
-    <t>calc_GR([12,22,28])</t>
-  </si>
-  <si>
-    <t>calc_PD([12,30,32],1)</t>
-  </si>
-  <si>
-    <t>calc_PD([12,30,32],2)</t>
-  </si>
-  <si>
-    <t>calc_PD([12,22,28],1)</t>
-  </si>
-  <si>
-    <t>calc_CD([12,30,32])</t>
-  </si>
-  <si>
-    <t>calc_CD([12,13,13,20])</t>
-  </si>
-  <si>
-    <t>calc_CD([12,20,20])</t>
-  </si>
-  <si>
-    <t>calc_incr_pos()</t>
-  </si>
-  <si>
-    <t>verify_gear_ratio(4+4/9,[12,20,32],[12,13,13,20],[12,20,20])</t>
-  </si>
-  <si>
-    <t>verify_gear_ratio(4+4/9,[12,20,32],[12,13,13,20],[12,20,99])</t>
-  </si>
-  <si>
-    <t>verify_gear_ratio(4+4/9,[12,20,32],[12,13,13,99],[12,20,20])</t>
-  </si>
-  <si>
-    <t>verify_gear_ratio(4+4/9,[12,20,32],[12,13,13,99],[12,99,99])</t>
-  </si>
-  <si>
-    <t>verify_center_distance(1,[12,20,32],[12,13,13,20],[12,20,20])</t>
-  </si>
-  <si>
-    <t>verify_center_distance(1,[12,20,32],[12,13,13,20],[12,99,20])</t>
-  </si>
-  <si>
-    <t>verify_center_distance(1,[12,20,32],[12,13,99,20],[12,20,20])</t>
-  </si>
-  <si>
-    <t>verify_center_distance(1,[12,20,99],[12,13,13,20],[12,20,20])</t>
-  </si>
-  <si>
-    <t>verify_center_distance(1,[12,20,32],[12,13,99,20],[12,99,20])</t>
-  </si>
-  <si>
-    <t>verify_center_distance(1,[12,20,99],[12,13,13,20],[12,99,20])</t>
-  </si>
-  <si>
-    <t>verify_center_distance(1,[12,20,99],[12,13,99,20],[12,20,20])</t>
-  </si>
-  <si>
-    <t>verify_center_distance(1,[12,20,99],[12,13,99,20],[12,99,20])</t>
-  </si>
-  <si>
-    <t>verify_center_distance(2,[12,20,32],[12,13,13,20],[12,20,20])</t>
-  </si>
-  <si>
-    <t>verify_center_distance(2,[6,10,16],[6,6.5,6.5,10],[6,10,10])</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,26 +320,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -274,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -297,101 +358,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -703,25 +685,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -743,159 +725,191 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>0.5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>0.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>0.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>0.5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>0.5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>0.5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>0.5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>0.5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>0.5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>0.5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C12">
         <v>0.5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <v>0.5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -907,94 +921,106 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="5" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>0.5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>0.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>0.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>0.5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>0.5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7" t="s">
         <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1002,43 +1028,55 @@
         <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>0.5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>0.5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>0.5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>0.5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1050,224 +1088,218 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="53.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="5" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>0.5</v>
       </c>
-      <c r="D2">
-        <v>1</v>
+      <c r="D2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>47</v>
+      <c r="A3" t="s">
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>0.5</v>
       </c>
-      <c r="D3">
-        <v>2</v>
+      <c r="D3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>48</v>
+      <c r="A4" t="s">
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>0.5</v>
       </c>
-      <c r="D4">
-        <v>3</v>
+      <c r="D4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>49</v>
+      <c r="A5" t="s">
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>0.5</v>
       </c>
-      <c r="D5">
-        <v>4</v>
+      <c r="D5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>0.5</v>
       </c>
-      <c r="D6">
-        <v>1</v>
+      <c r="D6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>51</v>
+      <c r="A7" t="s">
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>0.5</v>
       </c>
-      <c r="D7">
-        <v>2</v>
+      <c r="D7" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>52</v>
+      <c r="A8" t="s">
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>0.5</v>
       </c>
-      <c r="D8">
-        <v>3</v>
+      <c r="D8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>53</v>
+      <c r="A9" t="s">
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>0.5</v>
       </c>
-      <c r="D9">
-        <v>4</v>
+      <c r="D9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>54</v>
+      <c r="A10" t="s">
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>0.5</v>
       </c>
-      <c r="D10">
-        <v>5</v>
+      <c r="D10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>55</v>
+      <c r="A11" t="s">
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>0.5</v>
       </c>
-      <c r="D11">
-        <v>6</v>
+      <c r="D11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>56</v>
+      <c r="A12" t="s">
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>0.5</v>
       </c>
-      <c r="D12">
-        <v>7</v>
+      <c r="D12" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>57</v>
+      <c r="A13" t="s">
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>0.5</v>
       </c>
-      <c r="D13">
-        <v>8</v>
+      <c r="D13" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>58</v>
+      <c r="A14" t="s">
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>0.5</v>
       </c>
-      <c r="D14">
-        <v>8</v>
+      <c r="D14" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>59</v>
+      <c r="A15" t="s">
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>1.5</v>
       </c>
-      <c r="D15">
-        <v>1</v>
+      <c r="D15" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1279,40 +1311,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>0.5</v>
@@ -1323,38 +1348,38 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>0.5</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>0.5</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>0.5</v>
@@ -1365,41 +1390,41 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>0.5</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>0.5</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>0.25</v>
@@ -1407,10 +1432,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>0.5</v>
@@ -1421,10 +1446,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>0.25</v>
@@ -1432,10 +1457,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <v>0.5</v>
@@ -1446,10 +1471,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <v>0.5</v>

</xml_diff>

<commit_message>
Move scripts to a separate directory
</commit_message>
<xml_diff>
--- a/TestCases/MiniMilestone_TestCases.xlsx
+++ b/TestCases/MiniMilestone_TestCases.xlsx
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -50,6 +50,11 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -67,12 +72,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -101,10 +121,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -114,7 +137,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -490,19 +513,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="29" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="16.28515625" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
+    <col width="29" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="16.28515625" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="4">
-      <c r="A1" s="3" t="inlineStr">
+    <row r="1" ht="18.75" customHeight="1" s="5">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Guidelines for Inputs</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>Write inputs using Python syntax, passing in appropriate arguments to functions and methods</t>
         </is>
@@ -555,22 +578,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Command</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Outputs</t>
         </is>
@@ -856,22 +879,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Command</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Outputs</t>
         </is>
@@ -1097,22 +1120,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Command</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Outputs</t>
         </is>
@@ -1418,27 +1441,27 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Command</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>DontTest</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="E1" s="6" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>Outputs</t>
         </is>
@@ -1676,7 +1699,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>file="GivenFiles/test.txt"</t>
+          <t>file="../GivenFiles/test.txt"</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1721,7 +1744,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>file2="GivenFiles/write_test.txt"</t>
+          <t>file2="../GivenFiles/write_test.txt"</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">

</xml_diff>

<commit_message>
Move classes to a subdirectory
</commit_message>
<xml_diff>
--- a/TestCases/MiniMilestone_TestCases.xlsx
+++ b/TestCases/MiniMilestone_TestCases.xlsx
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -50,11 +50,6 @@
       <sz val="11"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -72,27 +67,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -121,13 +101,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -137,7 +114,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -513,19 +490,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="29" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
-    <col width="16.28515625" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="29" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
+    <col width="16.28515625" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="5">
-      <c r="A1" s="4" t="inlineStr">
+    <row r="1" ht="18.75" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Guidelines for Inputs</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="inlineStr">
+      <c r="A2" s="5" t="inlineStr">
         <is>
           <t>Write inputs using Python syntax, passing in appropriate arguments to functions and methods</t>
         </is>
@@ -578,22 +555,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Command</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Outputs</t>
         </is>
@@ -879,22 +856,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Command</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Outputs</t>
         </is>
@@ -1120,22 +1097,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Command</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Outputs</t>
         </is>
@@ -1441,27 +1418,27 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Command</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>DontTest</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>Outputs</t>
         </is>

</xml_diff>

<commit_message>
Revert "Move classes to a subdirectory"
This reverts commit 23522633
</commit_message>
<xml_diff>
--- a/TestCases/MiniMilestone_TestCases.xlsx
+++ b/TestCases/MiniMilestone_TestCases.xlsx
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -50,6 +50,11 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -67,12 +72,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -101,10 +121,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -114,7 +137,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -490,19 +513,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="29" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="16.28515625" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
+    <col width="29" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="16.28515625" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="4">
-      <c r="A1" s="3" t="inlineStr">
+    <row r="1" ht="18.75" customHeight="1" s="5">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Guidelines for Inputs</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>Write inputs using Python syntax, passing in appropriate arguments to functions and methods</t>
         </is>
@@ -555,22 +578,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Command</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Outputs</t>
         </is>
@@ -856,22 +879,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Command</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Outputs</t>
         </is>
@@ -1097,22 +1120,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Command</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Outputs</t>
         </is>
@@ -1418,27 +1441,27 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Command</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>DontTest</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="E1" s="6" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>Outputs</t>
         </is>

</xml_diff>